<commit_message>
progress has been made
</commit_message>
<xml_diff>
--- a/ablynxloader/src/main/resources/excels/People1 - Copy - Copy.xlsx
+++ b/ablynxloader/src/main/resources/excels/People1 - Copy - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="412">
   <si>
     <t>Michiel</t>
   </si>
@@ -1239,9 +1239,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>Jeroen</t>
-  </si>
-  <si>
     <t>doubles</t>
   </si>
   <si>
@@ -1255,6 +1252,15 @@
   </si>
   <si>
     <t>Rob</t>
+  </si>
+  <si>
+    <t>uh</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>nee</t>
   </si>
 </sst>
 </file>
@@ -1315,8 +1321,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="people" displayName="people" ref="E9:F11" totalsRowShown="0">
-  <autoFilter ref="E9:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="people" displayName="people" ref="E9:F13" totalsRowShown="0">
+  <autoFilter ref="E9:F13"/>
   <tableColumns count="2">
     <tableColumn id="1" name="first_name"/>
     <tableColumn id="2" name="age"/>
@@ -1588,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E9:F11"/>
+  <dimension ref="E9:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,10 +1620,26 @@
     </row>
     <row r="11" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="F11">
         <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>410</v>
+      </c>
+      <c r="F12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>411</v>
+      </c>
+      <c r="F13">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1632,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A9:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1660,10 +1682,10 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1671,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1684,7 +1706,7 @@
       </c>
       <c r="F10" s="1">
         <f ca="1" xml:space="preserve"> TODAY()</f>
-        <v>43006</v>
+        <v>43007</v>
       </c>
       <c r="G10" s="2">
         <v>0.19916165334139824</v>
@@ -1692,10 +1714,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1708,7 +1730,7 @@
       </c>
       <c r="F11" s="1">
         <f ca="1">F10+1</f>
-        <v>43007</v>
+        <v>43008</v>
       </c>
       <c r="G11" s="2">
         <v>0.4163163720275469</v>
@@ -1732,7 +1754,7 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" ref="F12:F75" ca="1" si="0">F11+1</f>
-        <v>43008</v>
+        <v>43009</v>
       </c>
       <c r="G12" s="2">
         <v>0.7163664606179394</v>
@@ -1756,7 +1778,7 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43009</v>
+        <v>43010</v>
       </c>
       <c r="G13" s="2">
         <v>0.48846370962378238</v>
@@ -1780,7 +1802,7 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43010</v>
+        <v>43011</v>
       </c>
       <c r="G14" s="2">
         <v>0.18293459937479883</v>
@@ -1804,7 +1826,7 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43011</v>
+        <v>43012</v>
       </c>
       <c r="G15" s="2">
         <v>0.55524867307877357</v>
@@ -1828,7 +1850,7 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43012</v>
+        <v>43013</v>
       </c>
       <c r="G16" s="2">
         <v>0.5119929521822979</v>
@@ -1852,7 +1874,7 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43013</v>
+        <v>43014</v>
       </c>
       <c r="G17" s="2">
         <v>0.61551073911253107</v>
@@ -1876,7 +1898,7 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43014</v>
+        <v>43015</v>
       </c>
       <c r="G18" s="2">
         <v>0.69497675934094494</v>
@@ -1900,7 +1922,7 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43015</v>
+        <v>43016</v>
       </c>
       <c r="G19" s="2">
         <v>0.45834359873746633</v>
@@ -1924,7 +1946,7 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43016</v>
+        <v>43017</v>
       </c>
       <c r="G20" s="2">
         <v>0.67759913711598718</v>
@@ -1948,7 +1970,7 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43017</v>
+        <v>43018</v>
       </c>
       <c r="G21" s="2">
         <v>0.52463956090917407</v>
@@ -1972,7 +1994,7 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43018</v>
+        <v>43019</v>
       </c>
       <c r="G22" s="2">
         <v>0.31030597290787143</v>
@@ -1996,7 +2018,7 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43019</v>
+        <v>43020</v>
       </c>
       <c r="G23" s="2">
         <v>0.42017830121998434</v>
@@ -2020,7 +2042,7 @@
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43020</v>
+        <v>43021</v>
       </c>
       <c r="G24" s="2">
         <v>0.46077178918196593</v>
@@ -2044,7 +2066,7 @@
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43021</v>
+        <v>43022</v>
       </c>
       <c r="G25" s="2">
         <v>0.32789172291650048</v>
@@ -2068,7 +2090,7 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43022</v>
+        <v>43023</v>
       </c>
       <c r="G26" s="2">
         <v>7.2552559483518575E-4</v>
@@ -2092,7 +2114,7 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43023</v>
+        <v>43024</v>
       </c>
       <c r="G27" s="2">
         <v>0.76249716396365153</v>
@@ -2116,7 +2138,7 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43024</v>
+        <v>43025</v>
       </c>
       <c r="G28" s="2">
         <v>0.3750071983009351</v>
@@ -2140,7 +2162,7 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43025</v>
+        <v>43026</v>
       </c>
       <c r="G29" s="2">
         <v>0.37846461641921336</v>
@@ -2164,7 +2186,7 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43026</v>
+        <v>43027</v>
       </c>
       <c r="G30" s="2">
         <v>0.96567931062216428</v>
@@ -2188,7 +2210,7 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43027</v>
+        <v>43028</v>
       </c>
       <c r="G31" s="2">
         <v>0.43091744996703851</v>
@@ -2212,7 +2234,7 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43028</v>
+        <v>43029</v>
       </c>
       <c r="G32" s="2">
         <v>0.64920230325149308</v>
@@ -2236,7 +2258,7 @@
       </c>
       <c r="F33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43029</v>
+        <v>43030</v>
       </c>
       <c r="G33" s="2">
         <v>0.85593790489185373</v>
@@ -2260,7 +2282,7 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43030</v>
+        <v>43031</v>
       </c>
       <c r="G34" s="2">
         <v>0.22852768403452484</v>
@@ -2284,7 +2306,7 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43031</v>
+        <v>43032</v>
       </c>
       <c r="G35" s="2">
         <v>0.16238606120812904</v>
@@ -2308,7 +2330,7 @@
       </c>
       <c r="F36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43032</v>
+        <v>43033</v>
       </c>
       <c r="G36" s="2">
         <v>0.53526087740902284</v>
@@ -2332,7 +2354,7 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43033</v>
+        <v>43034</v>
       </c>
       <c r="G37" s="2">
         <v>0.82194442761920605</v>
@@ -2356,7 +2378,7 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43034</v>
+        <v>43035</v>
       </c>
       <c r="G38" s="2">
         <v>0.88212965769788032</v>
@@ -2380,7 +2402,7 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43035</v>
+        <v>43036</v>
       </c>
       <c r="G39" s="2">
         <v>7.2250303799197169E-2</v>
@@ -2404,7 +2426,7 @@
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43036</v>
+        <v>43037</v>
       </c>
       <c r="G40" s="2">
         <v>7.1195702056510823E-2</v>
@@ -2428,7 +2450,7 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43037</v>
+        <v>43038</v>
       </c>
       <c r="G41" s="2">
         <v>0.85785120950915561</v>
@@ -2452,7 +2474,7 @@
       </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43038</v>
+        <v>43039</v>
       </c>
       <c r="G42" s="2">
         <v>0.30577153058324347</v>
@@ -2476,7 +2498,7 @@
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43039</v>
+        <v>43040</v>
       </c>
       <c r="G43" s="2">
         <v>0.31483526491145875</v>
@@ -2500,7 +2522,7 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43040</v>
+        <v>43041</v>
       </c>
       <c r="G44" s="2">
         <v>0.94599185402877539</v>
@@ -2524,7 +2546,7 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43041</v>
+        <v>43042</v>
       </c>
       <c r="G45" s="2">
         <v>0.34205280977493635</v>
@@ -2548,7 +2570,7 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43042</v>
+        <v>43043</v>
       </c>
       <c r="G46" s="2">
         <v>0.17705269996376227</v>
@@ -2572,7 +2594,7 @@
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43043</v>
+        <v>43044</v>
       </c>
       <c r="G47" s="2">
         <v>0.8731505416410984</v>
@@ -2596,7 +2618,7 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43044</v>
+        <v>43045</v>
       </c>
       <c r="G48" s="2">
         <v>3.4709672365056843E-2</v>
@@ -2620,7 +2642,7 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43045</v>
+        <v>43046</v>
       </c>
       <c r="G49" s="2">
         <v>0.56840793858086924</v>
@@ -2644,7 +2666,7 @@
       </c>
       <c r="F50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43046</v>
+        <v>43047</v>
       </c>
       <c r="G50" s="2">
         <v>0.66056676193295061</v>
@@ -2668,7 +2690,7 @@
       </c>
       <c r="F51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43047</v>
+        <v>43048</v>
       </c>
       <c r="G51" s="2">
         <v>0.9481936014422625</v>
@@ -2692,7 +2714,7 @@
       </c>
       <c r="F52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43048</v>
+        <v>43049</v>
       </c>
       <c r="G52" s="2">
         <v>0.48134481626866865</v>
@@ -2716,7 +2738,7 @@
       </c>
       <c r="F53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43049</v>
+        <v>43050</v>
       </c>
       <c r="G53" s="2">
         <v>0.98436272154419169</v>
@@ -2740,7 +2762,7 @@
       </c>
       <c r="F54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43050</v>
+        <v>43051</v>
       </c>
       <c r="G54" s="2">
         <v>0.24448855346001963</v>
@@ -2764,7 +2786,7 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43051</v>
+        <v>43052</v>
       </c>
       <c r="G55" s="2">
         <v>0.38813971210061615</v>
@@ -2788,7 +2810,7 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43052</v>
+        <v>43053</v>
       </c>
       <c r="G56" s="2">
         <v>0.18553229965365681</v>
@@ -2812,7 +2834,7 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43053</v>
+        <v>43054</v>
       </c>
       <c r="G57" s="2">
         <v>0.46398219265503382</v>
@@ -2836,7 +2858,7 @@
       </c>
       <c r="F58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43054</v>
+        <v>43055</v>
       </c>
       <c r="G58" s="2">
         <v>0.95347248750662683</v>
@@ -2860,7 +2882,7 @@
       </c>
       <c r="F59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43055</v>
+        <v>43056</v>
       </c>
       <c r="G59" s="2">
         <v>0.95523140993288003</v>
@@ -2884,7 +2906,7 @@
       </c>
       <c r="F60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43056</v>
+        <v>43057</v>
       </c>
       <c r="G60" s="2">
         <v>0.60285593026323092</v>
@@ -2908,7 +2930,7 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43057</v>
+        <v>43058</v>
       </c>
       <c r="G61" s="2">
         <v>0.80654472217638473</v>
@@ -2932,7 +2954,7 @@
       </c>
       <c r="F62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43058</v>
+        <v>43059</v>
       </c>
       <c r="G62" s="2">
         <v>0.23547687087211988</v>
@@ -2956,7 +2978,7 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43059</v>
+        <v>43060</v>
       </c>
       <c r="G63" s="2">
         <v>0.30970611241142176</v>
@@ -2980,7 +3002,7 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43060</v>
+        <v>43061</v>
       </c>
       <c r="G64" s="2">
         <v>0.28513850123847373</v>
@@ -3004,7 +3026,7 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43061</v>
+        <v>43062</v>
       </c>
       <c r="G65" s="2">
         <v>8.4540537865267495E-2</v>
@@ -3028,7 +3050,7 @@
       </c>
       <c r="F66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43062</v>
+        <v>43063</v>
       </c>
       <c r="G66" s="2">
         <v>0.7185829330697816</v>
@@ -3052,7 +3074,7 @@
       </c>
       <c r="F67" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43063</v>
+        <v>43064</v>
       </c>
       <c r="G67" s="2">
         <v>0.34062480906485459</v>
@@ -3076,7 +3098,7 @@
       </c>
       <c r="F68" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43064</v>
+        <v>43065</v>
       </c>
       <c r="G68" s="2">
         <v>0.17354261155111872</v>
@@ -3100,7 +3122,7 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43065</v>
+        <v>43066</v>
       </c>
       <c r="G69" s="2">
         <v>0.46191420869872024</v>
@@ -3124,7 +3146,7 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43066</v>
+        <v>43067</v>
       </c>
       <c r="G70" s="2">
         <v>0.98240017574459171</v>
@@ -3148,7 +3170,7 @@
       </c>
       <c r="F71" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43067</v>
+        <v>43068</v>
       </c>
       <c r="G71" s="2">
         <v>0.89474780241649521</v>
@@ -3172,7 +3194,7 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43068</v>
+        <v>43069</v>
       </c>
       <c r="G72" s="2">
         <v>0.21072742306706926</v>
@@ -3196,7 +3218,7 @@
       </c>
       <c r="F73" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43069</v>
+        <v>43070</v>
       </c>
       <c r="G73" s="2">
         <v>0.25434217867655362</v>
@@ -3220,7 +3242,7 @@
       </c>
       <c r="F74" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43070</v>
+        <v>43071</v>
       </c>
       <c r="G74" s="2">
         <v>0.35857915458283451</v>
@@ -3244,7 +3266,7 @@
       </c>
       <c r="F75" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43071</v>
+        <v>43072</v>
       </c>
       <c r="G75" s="2">
         <v>0.70109746172958098</v>
@@ -3268,7 +3290,7 @@
       </c>
       <c r="F76" s="1">
         <f t="shared" ref="F76:F109" ca="1" si="1">F75+1</f>
-        <v>43072</v>
+        <v>43073</v>
       </c>
       <c r="G76" s="2">
         <v>0.8471876752499663</v>
@@ -3292,7 +3314,7 @@
       </c>
       <c r="F77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43073</v>
+        <v>43074</v>
       </c>
       <c r="G77" s="2">
         <v>0.9301183879405106</v>
@@ -3316,7 +3338,7 @@
       </c>
       <c r="F78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43074</v>
+        <v>43075</v>
       </c>
       <c r="G78" s="2">
         <v>0.98862454976725322</v>
@@ -3340,7 +3362,7 @@
       </c>
       <c r="F79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43075</v>
+        <v>43076</v>
       </c>
       <c r="G79" s="2">
         <v>0.41342606802780646</v>
@@ -3364,7 +3386,7 @@
       </c>
       <c r="F80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43076</v>
+        <v>43077</v>
       </c>
       <c r="G80" s="2">
         <v>0.6252219871752509</v>
@@ -3388,7 +3410,7 @@
       </c>
       <c r="F81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43077</v>
+        <v>43078</v>
       </c>
       <c r="G81" s="2">
         <v>0.48873919776540264</v>
@@ -3412,7 +3434,7 @@
       </c>
       <c r="F82" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43078</v>
+        <v>43079</v>
       </c>
       <c r="G82" s="2">
         <v>9.3874144631708956E-2</v>
@@ -3436,7 +3458,7 @@
       </c>
       <c r="F83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43079</v>
+        <v>43080</v>
       </c>
       <c r="G83" s="2">
         <v>0.60362919914726854</v>
@@ -3460,7 +3482,7 @@
       </c>
       <c r="F84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43080</v>
+        <v>43081</v>
       </c>
       <c r="G84" s="2">
         <v>0.80739465754808015</v>
@@ -3484,7 +3506,7 @@
       </c>
       <c r="F85" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43081</v>
+        <v>43082</v>
       </c>
       <c r="G85" s="2">
         <v>0.24985761600844336</v>
@@ -3508,7 +3530,7 @@
       </c>
       <c r="F86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43082</v>
+        <v>43083</v>
       </c>
       <c r="G86" s="2">
         <v>0.73826040385492131</v>
@@ -3532,7 +3554,7 @@
       </c>
       <c r="F87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43083</v>
+        <v>43084</v>
       </c>
       <c r="G87" s="2">
         <v>0.70051873060312764</v>
@@ -3556,7 +3578,7 @@
       </c>
       <c r="F88" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43084</v>
+        <v>43085</v>
       </c>
       <c r="G88" s="2">
         <v>6.1603923952633366E-3</v>
@@ -3580,7 +3602,7 @@
       </c>
       <c r="F89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43085</v>
+        <v>43086</v>
       </c>
       <c r="G89" s="2">
         <v>0.31443172550467946</v>
@@ -3604,7 +3626,7 @@
       </c>
       <c r="F90" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43086</v>
+        <v>43087</v>
       </c>
       <c r="G90" s="2">
         <v>0.57097125794781001</v>
@@ -3628,7 +3650,7 @@
       </c>
       <c r="F91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43087</v>
+        <v>43088</v>
       </c>
       <c r="G91" s="2">
         <v>0.75931887043491542</v>
@@ -3652,7 +3674,7 @@
       </c>
       <c r="F92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43088</v>
+        <v>43089</v>
       </c>
       <c r="G92" s="2">
         <v>0.58467767595947751</v>
@@ -3676,7 +3698,7 @@
       </c>
       <c r="F93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43089</v>
+        <v>43090</v>
       </c>
       <c r="G93" s="2">
         <v>0.11403947277461057</v>
@@ -3700,7 +3722,7 @@
       </c>
       <c r="F94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43090</v>
+        <v>43091</v>
       </c>
       <c r="G94" s="2">
         <v>0.55355502971467729</v>
@@ -3724,7 +3746,7 @@
       </c>
       <c r="F95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43091</v>
+        <v>43092</v>
       </c>
       <c r="G95" s="2">
         <v>0.1638635460145611</v>
@@ -3748,7 +3770,7 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43092</v>
+        <v>43093</v>
       </c>
       <c r="G96" s="2">
         <v>0.51606244317239758</v>
@@ -3772,7 +3794,7 @@
       </c>
       <c r="F97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43093</v>
+        <v>43094</v>
       </c>
       <c r="G97" s="2">
         <v>0.48065729203617324</v>
@@ -3796,7 +3818,7 @@
       </c>
       <c r="F98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43094</v>
+        <v>43095</v>
       </c>
       <c r="G98" s="2">
         <v>0.83807925741546863</v>
@@ -3820,7 +3842,7 @@
       </c>
       <c r="F99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43095</v>
+        <v>43096</v>
       </c>
       <c r="G99" s="2">
         <v>0.50517143272725362</v>
@@ -3844,7 +3866,7 @@
       </c>
       <c r="F100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43096</v>
+        <v>43097</v>
       </c>
       <c r="G100" s="2">
         <v>0.14317582252941508</v>
@@ -3868,7 +3890,7 @@
       </c>
       <c r="F101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43097</v>
+        <v>43098</v>
       </c>
       <c r="G101" s="2">
         <v>0.21918409780116344</v>
@@ -3892,7 +3914,7 @@
       </c>
       <c r="F102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43098</v>
+        <v>43099</v>
       </c>
       <c r="G102" s="2">
         <v>0.31284191627988467</v>
@@ -3916,7 +3938,7 @@
       </c>
       <c r="F103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43099</v>
+        <v>43100</v>
       </c>
       <c r="G103" s="2">
         <v>0.99730369235531569</v>
@@ -3940,7 +3962,7 @@
       </c>
       <c r="F104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43100</v>
+        <v>43101</v>
       </c>
       <c r="G104" s="2">
         <v>0.84104753696091616</v>
@@ -3964,7 +3986,7 @@
       </c>
       <c r="F105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43101</v>
+        <v>43102</v>
       </c>
       <c r="G105" s="2">
         <v>0.85213043814510103</v>
@@ -3988,7 +4010,7 @@
       </c>
       <c r="F106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43102</v>
+        <v>43103</v>
       </c>
       <c r="G106" s="2">
         <v>0.17015790202817627</v>
@@ -4012,7 +4034,7 @@
       </c>
       <c r="F107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43103</v>
+        <v>43104</v>
       </c>
       <c r="G107" s="2">
         <v>0.31368438960705314</v>
@@ -4036,7 +4058,7 @@
       </c>
       <c r="F108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43104</v>
+        <v>43105</v>
       </c>
       <c r="G108" s="2">
         <v>0.27565930417431461</v>
@@ -4060,7 +4082,7 @@
       </c>
       <c r="F109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43105</v>
+        <v>43106</v>
       </c>
       <c r="G109" s="2">
         <v>0.93139807358768134</v>

</xml_diff>